<commit_message>
Doan day file de dam bao file moi nhat, ko can deploy file nao trong lan day nay
</commit_message>
<xml_diff>
--- a/2.Design/Template/Bieu_mau_hang_hoa.xlsx
+++ b/2.Design/Template/Bieu_mau_hang_hoa.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\2.DoanLV4_Document\LogDez\1.Document\WMS_Documents\2.Design\Template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2804CB18-10A7-418E-A7A6-B203370DE26C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88455BFE-24FF-4B14-B04E-52B1A889586C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -642,7 +642,7 @@
   <dimension ref="A1:L1"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -652,10 +652,11 @@
     <col min="3" max="3" width="25" customWidth="1"/>
     <col min="4" max="4" width="13.08984375" customWidth="1"/>
     <col min="5" max="5" width="11.1796875" customWidth="1"/>
-    <col min="6" max="6" width="10.54296875" customWidth="1"/>
+    <col min="6" max="6" width="10.08984375" customWidth="1"/>
     <col min="7" max="7" width="13.26953125" style="5" customWidth="1"/>
     <col min="8" max="8" width="12.90625" style="5" customWidth="1"/>
-    <col min="9" max="12" width="8.7265625" style="5"/>
+    <col min="9" max="9" width="8.6328125" style="5" customWidth="1"/>
+    <col min="10" max="12" width="8.7265625" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.35">

</xml_diff>